<commit_message>
changed extent report titles, added other fields of add user page
</commit_message>
<xml_diff>
--- a/src/main/java/com/qalegend/qa/testdata/exceldata.xlsx
+++ b/src/main/java/com/qalegend/qa/testdata/exceldata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -26,6 +26,48 @@
   </si>
   <si>
     <t>Athira</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Sales percent</t>
+  </si>
+  <si>
+    <t>anu123</t>
+  </si>
+  <si>
+    <t>mini123</t>
+  </si>
+  <si>
+    <t>athi123</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Executive</t>
+  </si>
+  <si>
+    <t>Specialist</t>
   </si>
 </sst>
 </file>
@@ -367,35 +409,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>